<commit_message>
Global flag for Report log
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/TestRunner.xlsx
+++ b/src/test/resources/Data/TestRunner.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\StarZPlay\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\StarZPlayAutomation\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37643B4B-E847-4646-AD98-77BF4BA59183}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618AE6B2-0D89-4703-9489-AB8F12ED51F4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{81C16DB0-A91E-4245-A63A-E0E19A862DCA}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="83">
   <si>
     <t>RunMode</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>landscape_poster_v1</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -680,7 +683,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,7 +780,7 @@
         <v>36</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>27</v>
@@ -815,7 +818,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>27</v>
@@ -850,7 +853,7 @@
         <v>59</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>28</v>
@@ -885,7 +888,7 @@
         <v>60</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>29</v>
@@ -920,7 +923,7 @@
         <v>72</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>30</v>
@@ -955,7 +958,7 @@
         <v>73</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>31</v>
@@ -990,7 +993,7 @@
         <v>75</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>32</v>
@@ -1025,7 +1028,7 @@
         <v>76</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>33</v>
@@ -1060,7 +1063,7 @@
         <v>61</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>34</v>
@@ -1095,7 +1098,7 @@
         <v>62</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>27</v>
@@ -1130,7 +1133,7 @@
         <v>55</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>28</v>
@@ -1165,7 +1168,7 @@
         <v>56</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>31</v>

</xml_diff>